<commit_message>
Permet le lancement avec N carrières
* Utilise pour COR2 de gen 1930 à gen 1990
</commit_message>
<xml_diff>
--- a/demo/carrieres.xlsx
+++ b/demo/carrieres.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="serie" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="debut" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -68,7 +69,13 @@
     <t xml:space="preserve">Cas type n°4 du COR (non cadre avec une interruption de carrière pour enfant)</t>
   </si>
   <si>
+    <t xml:space="preserve">PlafondSS</t>
+  </si>
+  <si>
     <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generation</t>
   </si>
 </sst>
 </file>
@@ -83,6 +90,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -168,10 +176,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,6 +262,17 @@
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -274,8 +293,8 @@
   </sheetPr>
   <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,7 +304,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>3</v>
@@ -2830,7 +2849,1088 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E62"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1930</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1931</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1932</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1933</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1934</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1935</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1936</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1937</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1938</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1939</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>1940</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1941</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1942</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>1943</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>1944</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>1945</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>1946</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>19.525</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>19.67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1947</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>19.341875</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>17.179375</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>17.179375</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>19.5725</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1948</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>19.15875</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>17.22875</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>17.22875</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>19.475</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1949</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>18.975625</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>17.278125</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>17.278125</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>19.3775</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1950</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>18.7925</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>17.3275</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>17.3275</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>19.28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1951</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>18.961875</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>17.4425</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>17.4425</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>19.38875</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>1952</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>19.13125</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>17.5575</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>17.5575</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>19.4975</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>1953</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>19.300625</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>17.6725</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>17.6725</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>19.60625</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>1954</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>19.47</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>17.7875</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>17.7875</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>19.715</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>1955</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>19.57625</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>17.898125</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>17.898125</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>19.81875</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>1956</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>19.6825</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>18.00875</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>18.00875</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>19.9225</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>1957</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>19.78875</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>18.119375</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>18.119375</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>20.02625</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>1958</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>19.895</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>18.23</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>18.23</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>20.13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>1959</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>18.328125</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>18.328125</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>20.249375</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>1960</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>20.085</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>18.42625</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>18.42625</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>20.36875</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>1961</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>20.18</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>18.524375</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>18.524375</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>20.488125</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>1962</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>20.275</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>18.6225</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>18.6225</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>20.6075</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>1963</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>20.40125</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>18.82625</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>18.82625</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>20.746875</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>1964</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>20.5275</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>19.03</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>19.03</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>20.88625</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>1965</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>20.65375</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>19.23375</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>19.23375</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>21.025625</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>1966</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>20.78</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>19.4375</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>19.4375</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>21.165</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>1967</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>20.90625</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>19.533125</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>19.533125</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>21.259375</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>1968</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>21.0325</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>19.62875</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>19.62875</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>21.35375</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>1969</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>21.15875</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>19.724375</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>19.724375</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>21.448125</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>1970</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>21.285</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>19.82</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>19.82</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>21.5425</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>1971</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>21.374375</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>19.990625</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>19.990625</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>21.656875</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>1972</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>21.46375</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>20.16125</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>20.16125</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>21.77125</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>1973</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>21.553125</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>20.331875</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>20.331875</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>21.885625</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>1974</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>21.6425</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>20.5025</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>20.5025</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>1975</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>21.645</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>20.538125</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>20.538125</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>21.95375</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>1976</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>21.6475</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>20.57375</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>20.57375</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>21.9075</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>1977</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>21.65</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>20.609375</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>20.609375</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>21.86125</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>1978</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>1979</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>1980</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>1981</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>1982</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>1983</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>1984</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>1985</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>1986</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>1987</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>1988</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>1989</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>1990</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>21.6525</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>20.645</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>21.815</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>